<commit_message>
changes ib ds and register
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestingData.xlsx
+++ b/src/test/resources/TestData/TestingData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dineshdeshmukh/eclipse-workspace/NinjaGalaxy-dsAlgo/src/test/resources/TestData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dineshdeshmukh/eclipse-workspace/TestNG/src/test/resources/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426C5663-4E9E-B345-9EF4-E6C0A437860C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BACB87F-EC4A-1642-8A3D-D0BE8840281B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" activeTab="2" xr2:uid="{C2348D72-976D-4F37-A81F-BEBD0C413FA4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" activeTab="1" xr2:uid="{C2348D72-976D-4F37-A81F-BEBD0C413FA4}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -46,9 +46,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>This is a test message !</t>
-  </si>
-  <si>
     <t>print('Python is fun!');</t>
   </si>
   <si>
@@ -165,6 +162,9 @@
   </si>
   <si>
     <t>Ninja_Galaxy20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	print('Hello</t>
   </si>
 </sst>
 </file>
@@ -613,19 +613,19 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -636,41 +636,41 @@
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="2"/>
     </row>
@@ -688,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EB5C662-2F1E-4CFF-8416-7834CF626327}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -699,17 +699,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -722,7 +722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4021EB5-FFC0-442B-8BA4-F9B02CB7FCEA}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -741,7 +741,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -751,45 +751,45 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>9</v>
       </c>
       <c r="C4" s="8"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>12</v>
-      </c>
       <c r="C6" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="8">
         <v>259603</v>
@@ -800,24 +800,24 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -845,23 +845,23 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="210" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="335" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -884,23 +884,23 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="112" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="192" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>